<commit_message>
Random setpoint tracking mpc initialised.
</commit_message>
<xml_diff>
--- a/Rough.xlsx
+++ b/Rough.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5585c3ced6b058bf/tu_d/Thesis/nmpc_cqr_gpu_thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{DD6046E6-DCDE-4837-860B-75522B57BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{28143E6C-873B-4471-BB4C-CF8DF54BF783}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{DD6046E6-DCDE-4837-860B-75522B57BBD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAE6203F-3B24-4820-B07F-53EDD0DCF1C4}"/>
   <bookViews>
-    <workbookView xWindow="5604" yWindow="-14988" windowWidth="17280" windowHeight="9420" xr2:uid="{81E51E6F-21B2-451B-B3E7-AC7E7D701810}"/>
+    <workbookView xWindow="-3540" yWindow="-17388" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{81E51E6F-21B2-451B-B3E7-AC7E7D701810}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -503,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4143AE3C-E94F-44D7-B389-830B823F7DA4}">
   <dimension ref="B4:R36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
@@ -1055,4 +1056,35 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66ACF574-7D7F-4D31-A456-E9C30B5E3D1C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>